<commit_message>
New start data cleaning
</commit_message>
<xml_diff>
--- a/data/ship_types.xlsx
+++ b/data/ship_types.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Fabia\Documents\GitHub\Thesis\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{440429D9-0045-4930-A6E6-73D3EF48D889}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBD61B59-4BB4-4142-B431-6FACA362F56C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{4F6C9A93-0C42-420E-A563-E317303BB045}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="50">
   <si>
     <t>RWS-class</t>
   </si>
@@ -143,6 +143,48 @@
   </si>
   <si>
     <t>BII-2L</t>
+  </si>
+  <si>
+    <t>CEMT-class</t>
+  </si>
+  <si>
+    <t>I</t>
+  </si>
+  <si>
+    <t>II</t>
+  </si>
+  <si>
+    <t>III</t>
+  </si>
+  <si>
+    <t>IVa</t>
+  </si>
+  <si>
+    <t>Va</t>
+  </si>
+  <si>
+    <t>VIa</t>
+  </si>
+  <si>
+    <t>IVb</t>
+  </si>
+  <si>
+    <t>Vb</t>
+  </si>
+  <si>
+    <t>VIb</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>IV</t>
+  </si>
+  <si>
+    <t>VIIa</t>
+  </si>
+  <si>
+    <t>VIc</t>
   </si>
 </sst>
 </file>
@@ -186,13 +228,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -507,15 +554,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB5155A1-C681-447D-9A50-1C8930620B11}">
-  <dimension ref="A1:C34"/>
+  <dimension ref="A1:D34"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30"/>
+      <selection activeCell="D34" sqref="A24:D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -525,14 +572,20 @@
       <c r="C1" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D1" s="7" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="4"/>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D2" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -542,8 +595,11 @@
       <c r="C3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D3" s="6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -554,8 +610,11 @@
         <f t="shared" ref="C4:C34" si="0">B4/$B$3</f>
         <v>1.7142857142857142</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D4" s="6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -566,8 +625,11 @@
         <f t="shared" si="0"/>
         <v>2.4857142857142858</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D5" s="6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -578,8 +640,11 @@
         <f t="shared" si="0"/>
         <v>2.4857142857142858</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D6" s="6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
@@ -590,8 +655,11 @@
         <f t="shared" si="0"/>
         <v>2.4857142857142858</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D7" s="6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
@@ -602,8 +670,11 @@
         <f t="shared" si="0"/>
         <v>3.9428571428571431</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D8" s="6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
@@ -614,8 +685,11 @@
         <f t="shared" si="0"/>
         <v>3.9428571428571431</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D9" s="6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
@@ -626,8 +700,11 @@
         <f t="shared" si="0"/>
         <v>8.1428571428571423</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D10" s="6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
@@ -638,8 +715,11 @@
         <f t="shared" si="0"/>
         <v>8.1428571428571423</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D11" s="6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
@@ -650,8 +730,11 @@
         <f t="shared" si="0"/>
         <v>11.514285714285714</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D12" s="6" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>12</v>
       </c>
@@ -662,8 +745,11 @@
         <f t="shared" si="0"/>
         <v>11.514285714285714</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D13" s="6" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>13</v>
       </c>
@@ -674,8 +760,11 @@
         <f t="shared" si="0"/>
         <v>11.514285714285714</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D14" s="6" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>14</v>
       </c>
@@ -686,8 +775,11 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D15" s="6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>15</v>
       </c>
@@ -698,8 +790,11 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D16" s="6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>16</v>
       </c>
@@ -710,8 +805,11 @@
         <f t="shared" si="0"/>
         <v>3.9428571428571431</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D17" s="6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>17</v>
       </c>
@@ -720,8 +818,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D18" s="6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>18</v>
       </c>
@@ -732,8 +833,11 @@
         <f t="shared" si="0"/>
         <v>11.514285714285714</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D19" s="6" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>19</v>
       </c>
@@ -744,8 +848,11 @@
         <f t="shared" si="0"/>
         <v>11.514285714285714</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D20" s="6" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>20</v>
       </c>
@@ -754,8 +861,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D21" s="6" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>31</v>
       </c>
@@ -766,8 +876,11 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D22" s="6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>32</v>
       </c>
@@ -778,8 +891,11 @@
         <f t="shared" si="0"/>
         <v>1.4285714285714286</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D23" s="6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>33</v>
       </c>
@@ -788,8 +904,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D24" s="6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>34</v>
       </c>
@@ -800,8 +919,11 @@
         <f t="shared" si="0"/>
         <v>2.4857142857142858</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D25" s="6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>21</v>
       </c>
@@ -812,8 +934,11 @@
         <f t="shared" si="0"/>
         <v>3.9428571428571431</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D26" s="6" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>22</v>
       </c>
@@ -824,8 +949,11 @@
         <f t="shared" si="0"/>
         <v>8.1428571428571423</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D27" s="6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>23</v>
       </c>
@@ -836,8 +964,11 @@
         <f t="shared" si="0"/>
         <v>8.1428571428571423</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D28" s="6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>24</v>
       </c>
@@ -848,8 +979,11 @@
         <f t="shared" si="0"/>
         <v>8.1428571428571423</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D29" s="6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>35</v>
       </c>
@@ -858,8 +992,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D30" s="6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>25</v>
       </c>
@@ -870,8 +1007,11 @@
         <f t="shared" si="0"/>
         <v>11.514285714285714</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D31" s="6" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>26</v>
       </c>
@@ -880,8 +1020,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D32" s="6" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>27</v>
       </c>
@@ -889,14 +1032,20 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D33" s="6" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C34" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
+      </c>
+      <c r="D34" s="6" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Additional analysis route selection, setup to try top 200 flows instead of top 100 routes
</commit_message>
<xml_diff>
--- a/data/ship_types.xlsx
+++ b/data/ship_types.xlsx
@@ -461,12 +461,12 @@
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
+          <t>battery_size</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
           <t>Factor</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>battery_size</t>
         </is>
       </c>
     </row>
@@ -494,10 +494,10 @@
         </is>
       </c>
       <c r="G2" t="n">
+        <v>946.0482214293436</v>
+      </c>
+      <c r="H2" t="n">
         <v>5.405989836739106</v>
-      </c>
-      <c r="H2" t="n">
-        <v>946.0482214293436</v>
       </c>
     </row>
     <row r="3">
@@ -524,10 +524,10 @@
         </is>
       </c>
       <c r="G3" t="n">
+        <v>1239.710403649707</v>
+      </c>
+      <c r="H3" t="n">
         <v>7.084059449426899</v>
-      </c>
-      <c r="H3" t="n">
-        <v>1239.710403649707</v>
       </c>
     </row>
     <row r="4">
@@ -554,10 +554,10 @@
         </is>
       </c>
       <c r="G4" t="n">
+        <v>1877.751877751878</v>
+      </c>
+      <c r="H4" t="n">
         <v>10.73001073001073</v>
-      </c>
-      <c r="H4" t="n">
-        <v>1877.751877751878</v>
       </c>
     </row>
     <row r="5">
@@ -584,10 +584,10 @@
         </is>
       </c>
       <c r="G5" t="n">
+        <v>1812.5</v>
+      </c>
+      <c r="H5" t="n">
         <v>10.35714285714286</v>
-      </c>
-      <c r="H5" t="n">
-        <v>1812.5</v>
       </c>
     </row>
     <row r="6">
@@ -614,10 +614,10 @@
         </is>
       </c>
       <c r="G6" t="n">
+        <v>1851.378958120531</v>
+      </c>
+      <c r="H6" t="n">
         <v>10.57930833211732</v>
-      </c>
-      <c r="H6" t="n">
-        <v>1851.378958120531</v>
       </c>
     </row>
     <row r="7">
@@ -644,10 +644,10 @@
         </is>
       </c>
       <c r="G7" t="n">
+        <v>2936.670071501532</v>
+      </c>
+      <c r="H7" t="n">
         <v>16.78097183715161</v>
-      </c>
-      <c r="H7" t="n">
-        <v>2936.670071501532</v>
       </c>
     </row>
     <row r="8">
@@ -674,10 +674,10 @@
         </is>
       </c>
       <c r="G8" t="n">
+        <v>3043.938591847539</v>
+      </c>
+      <c r="H8" t="n">
         <v>17.39393481055737</v>
-      </c>
-      <c r="H8" t="n">
-        <v>3043.938591847539</v>
       </c>
     </row>
     <row r="9">
@@ -704,10 +704,10 @@
         </is>
       </c>
       <c r="G9" t="n">
+        <v>5982.476109802261</v>
+      </c>
+      <c r="H9" t="n">
         <v>34.18557777029864</v>
-      </c>
-      <c r="H9" t="n">
-        <v>5982.476109802261</v>
       </c>
     </row>
     <row r="10">
@@ -734,10 +734,10 @@
         </is>
       </c>
       <c r="G10" t="n">
+        <v>7639.071397284275</v>
+      </c>
+      <c r="H10" t="n">
         <v>43.65183655591014</v>
-      </c>
-      <c r="H10" t="n">
-        <v>7639.071397284275</v>
       </c>
     </row>
     <row r="11">
@@ -764,10 +764,10 @@
         </is>
       </c>
       <c r="G11" t="n">
+        <v>7670.480974974415</v>
+      </c>
+      <c r="H11" t="n">
         <v>43.83131985699666</v>
-      </c>
-      <c r="H11" t="n">
-        <v>7670.480974974415</v>
       </c>
     </row>
     <row r="12">
@@ -794,10 +794,10 @@
         </is>
       </c>
       <c r="G12" t="n">
+        <v>8364.373810115057</v>
+      </c>
+      <c r="H12" t="n">
         <v>47.79642177208604</v>
-      </c>
-      <c r="H12" t="n">
-        <v>8364.373810115057</v>
       </c>
     </row>
     <row r="13">
@@ -824,10 +824,10 @@
         </is>
       </c>
       <c r="G13" t="n">
+        <v>9572.187928669409</v>
+      </c>
+      <c r="H13" t="n">
         <v>54.69821673525377</v>
-      </c>
-      <c r="H13" t="n">
-        <v>9572.187928669409</v>
       </c>
     </row>
     <row r="14">
@@ -854,10 +854,10 @@
         </is>
       </c>
       <c r="G14" t="n">
+        <v>428.5591840233137</v>
+      </c>
+      <c r="H14" t="n">
         <v>2.448909622990364</v>
-      </c>
-      <c r="H14" t="n">
-        <v>428.5591840233137</v>
       </c>
     </row>
     <row r="15">
@@ -884,10 +884,10 @@
         </is>
       </c>
       <c r="G15" t="n">
+        <v>600.0600060006</v>
+      </c>
+      <c r="H15" t="n">
         <v>3.428914320003428</v>
-      </c>
-      <c r="H15" t="n">
-        <v>600.0600060006</v>
       </c>
     </row>
     <row r="16">
@@ -914,10 +914,10 @@
         </is>
       </c>
       <c r="G16" t="n">
+        <v>681.7562039814561</v>
+      </c>
+      <c r="H16" t="n">
         <v>3.895749737036892</v>
-      </c>
-      <c r="H16" t="n">
-        <v>681.7562039814561</v>
       </c>
     </row>
     <row r="17">
@@ -944,10 +944,10 @@
         </is>
       </c>
       <c r="G17" t="n">
+        <v>1676.371978118934</v>
+      </c>
+      <c r="H17" t="n">
         <v>9.579268446393911</v>
-      </c>
-      <c r="H17" t="n">
-        <v>1676.371978118934</v>
       </c>
     </row>
     <row r="18">
@@ -974,10 +974,10 @@
         </is>
       </c>
       <c r="G18" t="n">
+        <v>3355.155482815057</v>
+      </c>
+      <c r="H18" t="n">
         <v>19.17231704465747</v>
-      </c>
-      <c r="H18" t="n">
-        <v>3355.155482815057</v>
       </c>
     </row>
     <row r="19">
@@ -1004,10 +1004,10 @@
         </is>
       </c>
       <c r="G19" t="n">
+        <v>5804.031879981248</v>
+      </c>
+      <c r="H19" t="n">
         <v>33.1658964570357</v>
-      </c>
-      <c r="H19" t="n">
-        <v>5804.031879981248</v>
       </c>
     </row>
     <row r="20">
@@ -1034,10 +1034,10 @@
         </is>
       </c>
       <c r="G20" t="n">
+        <v>5671.614440168591</v>
+      </c>
+      <c r="H20" t="n">
         <v>32.40922537239194</v>
-      </c>
-      <c r="H20" t="n">
-        <v>5671.614440168591</v>
       </c>
     </row>
     <row r="21">
@@ -1064,10 +1064,10 @@
         </is>
       </c>
       <c r="G21" t="n">
+        <v>6753.955264593562</v>
+      </c>
+      <c r="H21" t="n">
         <v>38.59403008339178</v>
-      </c>
-      <c r="H21" t="n">
-        <v>6753.955264593562</v>
       </c>
     </row>
     <row r="22">
@@ -1094,10 +1094,10 @@
         </is>
       </c>
       <c r="G22" t="n">
+        <v>7283.209789386986</v>
+      </c>
+      <c r="H22" t="n">
         <v>41.61834165363992</v>
-      </c>
-      <c r="H22" t="n">
-        <v>7283.209789386986</v>
       </c>
     </row>
     <row r="23">
@@ -1124,10 +1124,10 @@
         </is>
       </c>
       <c r="G23" t="n">
+        <v>7736.532933383326</v>
+      </c>
+      <c r="H23" t="n">
         <v>44.20875961933329</v>
-      </c>
-      <c r="H23" t="n">
-        <v>7736.532933383326</v>
       </c>
     </row>
     <row r="24">
@@ -1154,10 +1154,10 @@
         </is>
       </c>
       <c r="G24" t="n">
+        <v>7736.532933383326</v>
+      </c>
+      <c r="H24" t="n">
         <v>44.20875961933329</v>
-      </c>
-      <c r="H24" t="n">
-        <v>7736.532933383326</v>
       </c>
     </row>
     <row r="25">
@@ -1184,10 +1184,10 @@
         </is>
       </c>
       <c r="G25" t="n">
+        <v>889.7701850721985</v>
+      </c>
+      <c r="H25" t="n">
         <v>5.08440105755542</v>
-      </c>
-      <c r="H25" t="n">
-        <v>889.7701850721985</v>
       </c>
     </row>
     <row r="26">
@@ -1214,10 +1214,10 @@
         </is>
       </c>
       <c r="G26" t="n">
+        <v>972.2222222222222</v>
+      </c>
+      <c r="H26" t="n">
         <v>5.555555555555555</v>
-      </c>
-      <c r="H26" t="n">
-        <v>972.2222222222222</v>
       </c>
     </row>
     <row r="27">
@@ -1244,10 +1244,10 @@
         </is>
       </c>
       <c r="G27" t="n">
+        <v>3209.600893106335</v>
+      </c>
+      <c r="H27" t="n">
         <v>18.3405765320362</v>
-      </c>
-      <c r="H27" t="n">
-        <v>3209.600893106335</v>
       </c>
     </row>
     <row r="28">
@@ -1274,10 +1274,10 @@
         </is>
       </c>
       <c r="G28" t="n">
+        <v>7307.692307692307</v>
+      </c>
+      <c r="H28" t="n">
         <v>41.75824175824175</v>
-      </c>
-      <c r="H28" t="n">
-        <v>7307.692307692307</v>
       </c>
     </row>
     <row r="29">
@@ -1304,10 +1304,10 @@
         </is>
       </c>
       <c r="G29" t="n">
+        <v>4452.187379016647</v>
+      </c>
+      <c r="H29" t="n">
         <v>25.44107073723799</v>
-      </c>
-      <c r="H29" t="n">
-        <v>4452.187379016647</v>
       </c>
     </row>
     <row r="30">
@@ -1334,10 +1334,10 @@
         </is>
       </c>
       <c r="G30" t="n">
+        <v>10180.02571795971</v>
+      </c>
+      <c r="H30" t="n">
         <v>58.17157553119832</v>
-      </c>
-      <c r="H30" t="n">
-        <v>10180.02571795971</v>
       </c>
     </row>
     <row r="31">
@@ -1364,10 +1364,10 @@
         </is>
       </c>
       <c r="G31" t="n">
+        <v>7916.666666666666</v>
+      </c>
+      <c r="H31" t="n">
         <v>45.23809523809523</v>
-      </c>
-      <c r="H31" t="n">
-        <v>7916.666666666666</v>
       </c>
     </row>
     <row r="32">
@@ -1394,10 +1394,10 @@
         </is>
       </c>
       <c r="G32" t="n">
+        <v>6680.731364275668</v>
+      </c>
+      <c r="H32" t="n">
         <v>38.17560779586096</v>
-      </c>
-      <c r="H32" t="n">
-        <v>6680.731364275668</v>
       </c>
     </row>
     <row r="33">
@@ -1424,10 +1424,10 @@
         </is>
       </c>
       <c r="G33" t="n">
+        <v>6680.731364275668</v>
+      </c>
+      <c r="H33" t="n">
         <v>38.17560779586096</v>
-      </c>
-      <c r="H33" t="n">
-        <v>6680.731364275668</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
flow factors fixed + new run ABM
</commit_message>
<xml_diff>
--- a/data/ship_types.xlsx
+++ b/data/ship_types.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H33"/>
+  <dimension ref="A1:I33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -461,12 +461,17 @@
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>battery_size</t>
+          <t>battery_size_70000</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>Factor</t>
+          <t>battery_size_110000</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>battery_size_150000</t>
         </is>
       </c>
     </row>
@@ -494,10 +499,13 @@
         </is>
       </c>
       <c r="G2" t="n">
-        <v>946.0482214293436</v>
+        <v>1103.722925000901</v>
       </c>
       <c r="H2" t="n">
-        <v>1</v>
+        <v>1734.42173928713</v>
+      </c>
+      <c r="I2" t="n">
+        <v>2365.120553573359</v>
       </c>
     </row>
     <row r="3">
@@ -524,10 +532,13 @@
         </is>
       </c>
       <c r="G3" t="n">
-        <v>1239.710403649707</v>
+        <v>1446.328804257992</v>
       </c>
       <c r="H3" t="n">
-        <v>1.310409316954988</v>
+        <v>2272.80240669113</v>
+      </c>
+      <c r="I3" t="n">
+        <v>3099.276009124269</v>
       </c>
     </row>
     <row r="4">
@@ -554,10 +565,13 @@
         </is>
       </c>
       <c r="G4" t="n">
-        <v>1877.751877751878</v>
+        <v>2190.710524043857</v>
       </c>
       <c r="H4" t="n">
-        <v>1.984837384837385</v>
+        <v>3442.545109211776</v>
+      </c>
+      <c r="I4" t="n">
+        <v>4694.379694379693</v>
       </c>
     </row>
     <row r="5">
@@ -584,10 +598,13 @@
         </is>
       </c>
       <c r="G5" t="n">
-        <v>1812.5</v>
+        <v>2114.583333333333</v>
       </c>
       <c r="H5" t="n">
-        <v>1.915864285714286</v>
+        <v>3322.916666666667</v>
+      </c>
+      <c r="I5" t="n">
+        <v>4531.25</v>
       </c>
     </row>
     <row r="6">
@@ -614,10 +631,13 @@
         </is>
       </c>
       <c r="G6" t="n">
-        <v>1851.378958120531</v>
+        <v>2159.942117807286</v>
       </c>
       <c r="H6" t="n">
-        <v>1.956960455275062</v>
+        <v>3394.194756554307</v>
+      </c>
+      <c r="I6" t="n">
+        <v>4628.447395301328</v>
       </c>
     </row>
     <row r="7">
@@ -644,10 +664,13 @@
         </is>
       </c>
       <c r="G7" t="n">
-        <v>2936.670071501532</v>
+        <v>3426.115083418454</v>
       </c>
       <c r="H7" t="n">
-        <v>3.104144170436306</v>
+        <v>5383.895131086142</v>
+      </c>
+      <c r="I7" t="n">
+        <v>7341.675178753831</v>
       </c>
     </row>
     <row r="8">
@@ -674,10 +697,13 @@
         </is>
       </c>
       <c r="G8" t="n">
-        <v>3043.938591847539</v>
+        <v>3551.261690488795</v>
       </c>
       <c r="H8" t="n">
-        <v>3.217530061256902</v>
+        <v>5580.55408505382</v>
+      </c>
+      <c r="I8" t="n">
+        <v>7609.846479618847</v>
       </c>
     </row>
     <row r="9">
@@ -704,10 +730,13 @@
         </is>
       </c>
       <c r="G9" t="n">
-        <v>5982.476109802261</v>
+        <v>6979.555461435971</v>
       </c>
       <c r="H9" t="n">
-        <v>6.323648175949842</v>
+        <v>10967.87286797081</v>
+      </c>
+      <c r="I9" t="n">
+        <v>14956.19027450565</v>
       </c>
     </row>
     <row r="10">
@@ -734,10 +763,13 @@
         </is>
       </c>
       <c r="G10" t="n">
-        <v>7639.071397284275</v>
+        <v>8912.249963498321</v>
       </c>
       <c r="H10" t="n">
-        <v>8.074716726112259</v>
+        <v>14004.9642283545</v>
+      </c>
+      <c r="I10" t="n">
+        <v>19097.67849321069</v>
       </c>
     </row>
     <row r="11">
@@ -764,10 +796,13 @@
         </is>
       </c>
       <c r="G11" t="n">
-        <v>7670.480974974415</v>
+        <v>8948.894470803485</v>
       </c>
       <c r="H11" t="n">
-        <v>8.107917547147244</v>
+        <v>14062.54845411976</v>
+      </c>
+      <c r="I11" t="n">
+        <v>19176.20243743604</v>
       </c>
     </row>
     <row r="12">
@@ -794,10 +829,13 @@
         </is>
       </c>
       <c r="G12" t="n">
-        <v>8364.373810115057</v>
+        <v>9758.4361118009</v>
       </c>
       <c r="H12" t="n">
-        <v>8.841382099400477</v>
+        <v>15334.68531854427</v>
+      </c>
+      <c r="I12" t="n">
+        <v>20910.93452528764</v>
       </c>
     </row>
     <row r="13">
@@ -824,10 +862,13 @@
         </is>
       </c>
       <c r="G13" t="n">
-        <v>9572.187928669409</v>
+        <v>11167.55258344764</v>
       </c>
       <c r="H13" t="n">
-        <v>10.11807613168724</v>
+        <v>17549.01120256058</v>
+      </c>
+      <c r="I13" t="n">
+        <v>23930.46982167352</v>
       </c>
     </row>
     <row r="14">
@@ -854,10 +895,13 @@
         </is>
       </c>
       <c r="G14" t="n">
-        <v>428.5591840233137</v>
+        <v>499.9857146938659</v>
       </c>
       <c r="H14" t="n">
-        <v>0.4529993020607576</v>
+        <v>785.691837376075</v>
+      </c>
+      <c r="I14" t="n">
+        <v>1071.397960058284</v>
       </c>
     </row>
     <row r="15">
@@ -884,10 +928,13 @@
         </is>
       </c>
       <c r="G15" t="n">
-        <v>600.0600060006</v>
+        <v>700.0700070007</v>
       </c>
       <c r="H15" t="n">
-        <v>0.6342805709142343</v>
+        <v>1100.1100110011</v>
+      </c>
+      <c r="I15" t="n">
+        <v>1500.1500150015</v>
       </c>
     </row>
     <row r="16">
@@ -914,10 +961,13 @@
         </is>
       </c>
       <c r="G16" t="n">
-        <v>681.7562039814561</v>
+        <v>795.3822379783657</v>
       </c>
       <c r="H16" t="n">
-        <v>0.7206357863570844</v>
+        <v>1249.886373966003</v>
+      </c>
+      <c r="I16" t="n">
+        <v>1704.390509953641</v>
       </c>
     </row>
     <row r="17">
@@ -944,10 +994,13 @@
         </is>
       </c>
       <c r="G17" t="n">
-        <v>1676.371978118934</v>
+        <v>1955.767307805423</v>
       </c>
       <c r="H17" t="n">
-        <v>1.771973077213946</v>
+        <v>3073.348626551379</v>
+      </c>
+      <c r="I17" t="n">
+        <v>4190.929945297336</v>
       </c>
     </row>
     <row r="18">
@@ -974,10 +1027,13 @@
         </is>
       </c>
       <c r="G18" t="n">
-        <v>3355.155482815057</v>
+        <v>3914.348063284233</v>
       </c>
       <c r="H18" t="n">
-        <v>3.546495206920739</v>
+        <v>6151.118385160938</v>
+      </c>
+      <c r="I18" t="n">
+        <v>8387.888707037642</v>
       </c>
     </row>
     <row r="19">
@@ -1004,10 +1060,13 @@
         </is>
       </c>
       <c r="G19" t="n">
-        <v>5804.031879981248</v>
+        <v>6771.370526644788</v>
       </c>
       <c r="H19" t="n">
-        <v>6.135027526622465</v>
+        <v>10640.72511329895</v>
+      </c>
+      <c r="I19" t="n">
+        <v>14510.07969995312</v>
       </c>
     </row>
     <row r="20">
@@ -1034,10 +1093,13 @@
         </is>
       </c>
       <c r="G20" t="n">
-        <v>5671.614440168591</v>
+        <v>6616.883513530022</v>
       </c>
       <c r="H20" t="n">
-        <v>5.995058509385063</v>
+        <v>10397.95980697575</v>
+      </c>
+      <c r="I20" t="n">
+        <v>14179.03610042148</v>
       </c>
     </row>
     <row r="21">
@@ -1064,10 +1126,13 @@
         </is>
       </c>
       <c r="G21" t="n">
-        <v>6753.955264593562</v>
+        <v>7879.614475359155</v>
       </c>
       <c r="H21" t="n">
-        <v>7.139123684825813</v>
+        <v>12382.25131842153</v>
+      </c>
+      <c r="I21" t="n">
+        <v>16884.8881614839</v>
       </c>
     </row>
     <row r="22">
@@ -1094,10 +1159,13 @@
         </is>
       </c>
       <c r="G22" t="n">
-        <v>7283.209789386986</v>
+        <v>8497.078087618151</v>
       </c>
       <c r="H22" t="n">
-        <v>7.698560839090313</v>
+        <v>13352.55128054281</v>
+      </c>
+      <c r="I22" t="n">
+        <v>18208.02447346747</v>
       </c>
     </row>
     <row r="23">
@@ -1124,10 +1192,13 @@
         </is>
       </c>
       <c r="G23" t="n">
-        <v>7736.532933383326</v>
+        <v>9025.955088947214</v>
       </c>
       <c r="H23" t="n">
-        <v>8.177736354384274</v>
+        <v>14183.64371120277</v>
+      </c>
+      <c r="I23" t="n">
+        <v>19341.33233345831</v>
       </c>
     </row>
     <row r="24">
@@ -1154,10 +1225,13 @@
         </is>
       </c>
       <c r="G24" t="n">
-        <v>7736.532933383326</v>
+        <v>9025.955088947214</v>
       </c>
       <c r="H24" t="n">
-        <v>8.177736354384274</v>
+        <v>14183.64371120277</v>
+      </c>
+      <c r="I24" t="n">
+        <v>19341.33233345831</v>
       </c>
     </row>
     <row r="25">
@@ -1184,10 +1258,13 @@
         </is>
       </c>
       <c r="G25" t="n">
-        <v>889.7701850721985</v>
+        <v>1038.065215917565</v>
       </c>
       <c r="H25" t="n">
-        <v>0.9405125076266018</v>
+        <v>1631.245339299031</v>
+      </c>
+      <c r="I25" t="n">
+        <v>2224.425462680496</v>
       </c>
     </row>
     <row r="26">
@@ -1214,10 +1291,13 @@
         </is>
       </c>
       <c r="G26" t="n">
-        <v>972.2222222222222</v>
+        <v>1134.259259259259</v>
       </c>
       <c r="H26" t="n">
-        <v>1.027666666666667</v>
+        <v>1782.407407407407</v>
+      </c>
+      <c r="I26" t="n">
+        <v>2430.555555555556</v>
       </c>
     </row>
     <row r="27">
@@ -1244,10 +1324,13 @@
         </is>
       </c>
       <c r="G27" t="n">
-        <v>3209.600893106335</v>
+        <v>3744.534375290724</v>
       </c>
       <c r="H27" t="n">
-        <v>3.392639846896057</v>
+        <v>5884.268304028282</v>
+      </c>
+      <c r="I27" t="n">
+        <v>8024.002232765838</v>
       </c>
     </row>
     <row r="28">
@@ -1274,10 +1357,13 @@
         </is>
       </c>
       <c r="G28" t="n">
-        <v>7307.692307692307</v>
+        <v>8525.641025641024</v>
       </c>
       <c r="H28" t="n">
-        <v>7.724439560439561</v>
+        <v>13397.43589743589</v>
+      </c>
+      <c r="I28" t="n">
+        <v>18269.23076923077</v>
       </c>
     </row>
     <row r="29">
@@ -1304,10 +1390,13 @@
         </is>
       </c>
       <c r="G29" t="n">
-        <v>4452.187379016647</v>
+        <v>5194.218608852754</v>
       </c>
       <c r="H29" t="n">
-        <v>4.706089264974283</v>
+        <v>8162.343528197185</v>
+      </c>
+      <c r="I29" t="n">
+        <v>11130.46844754162</v>
       </c>
     </row>
     <row r="30">
@@ -1334,10 +1423,13 @@
         </is>
       </c>
       <c r="G30" t="n">
-        <v>10180.02571795971</v>
+        <v>11876.69667095299</v>
       </c>
       <c r="H30" t="n">
-        <v>10.76057804176107</v>
+        <v>18663.38048292613</v>
+      </c>
+      <c r="I30" t="n">
+        <v>25450.06429489927</v>
       </c>
     </row>
     <row r="31">
@@ -1364,10 +1456,13 @@
         </is>
       </c>
       <c r="G31" t="n">
-        <v>7916.666666666666</v>
+        <v>9236.111111111111</v>
       </c>
       <c r="H31" t="n">
-        <v>8.368142857142857</v>
+        <v>14513.88888888889</v>
+      </c>
+      <c r="I31" t="n">
+        <v>19791.66666666667</v>
       </c>
     </row>
     <row r="32">
@@ -1394,10 +1489,13 @@
         </is>
       </c>
       <c r="G32" t="n">
-        <v>6680.731364275668</v>
+        <v>7794.186591654946</v>
       </c>
       <c r="H32" t="n">
-        <v>7.061723930078362</v>
+        <v>12248.00750117206</v>
+      </c>
+      <c r="I32" t="n">
+        <v>16701.82841068917</v>
       </c>
     </row>
     <row r="33">
@@ -1424,10 +1522,13 @@
         </is>
       </c>
       <c r="G33" t="n">
-        <v>6680.731364275668</v>
+        <v>7794.186591654946</v>
       </c>
       <c r="H33" t="n">
-        <v>7.061723930078362</v>
+        <v>12248.00750117206</v>
+      </c>
+      <c r="I33" t="n">
+        <v>16701.82841068917</v>
       </c>
     </row>
   </sheetData>

</xml_diff>